<commit_message>
Updated Cost Estimate Analysis.xlsx & Cost Management Plan_MLNSD.docx
</commit_message>
<xml_diff>
--- a/documentation/projman/Cost Estimate Analysis.xlsx
+++ b/documentation/projman/Cost Estimate Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\APC_2022_2023_T3_PROJMAN_MI201_MI203_G03_Team_MLNSD\documentation\projman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B118D40-3ADD-4DC7-AAA4-827DB8A263C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3598DDFF-62B9-4643-8B7E-08F8C9A83AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5580" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{B4D77BE3-67E7-4318-A3E5-40FCD1C2165C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Total Cost</t>
   </si>
@@ -86,15 +86,6 @@
     <t>Deployment/Platform</t>
   </si>
   <si>
-    <t>Web Hosting</t>
-  </si>
-  <si>
-    <t>SSL Security</t>
-  </si>
-  <si>
-    <t>Domain Registration</t>
-  </si>
-  <si>
     <t>Equipment</t>
   </si>
   <si>
@@ -132,6 +123,21 @@
   </si>
   <si>
     <t>Indirect Cost</t>
+  </si>
+  <si>
+    <t>Actual Cost</t>
+  </si>
+  <si>
+    <t>Rental (10% of Depreciated Value)</t>
+  </si>
+  <si>
+    <t>Web Hosting (GoDaddy)</t>
+  </si>
+  <si>
+    <t>SSL Security (GoDaddy)</t>
+  </si>
+  <si>
+    <t>Domain Registration  (GoDaddy)</t>
   </si>
 </sst>
 </file>
@@ -350,7 +356,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -378,7 +384,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
@@ -409,6 +414,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -729,17 +737,17 @@
   </sheetPr>
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="37.73046875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.9296875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.46484375" bestFit="1" customWidth="1"/>
   </cols>
@@ -763,32 +771,32 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="28"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="27"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="7" t="s">
@@ -801,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" s="7" t="s">
         <v>5</v>
@@ -873,11 +881,15 @@
       <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="17"/>
+      <c r="C9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>30</v>
+      </c>
       <c r="F9" s="14" t="s">
         <v>0</v>
       </c>
@@ -887,14 +899,16 @@
         <v>15</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="18"/>
-      <c r="D10" s="21">
+        <v>31</v>
+      </c>
+      <c r="C10" s="31">
+        <v>5988</v>
+      </c>
+      <c r="D10" s="20">
         <v>1</v>
       </c>
       <c r="E10" s="18"/>
-      <c r="F10" s="22">
+      <c r="F10" s="21">
         <v>5988</v>
       </c>
     </row>
@@ -903,14 +917,16 @@
         <v>15</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21">
+        <v>32</v>
+      </c>
+      <c r="C11" s="31">
+        <v>7999</v>
+      </c>
+      <c r="D11" s="20">
         <v>1</v>
       </c>
       <c r="E11" s="18"/>
-      <c r="F11" s="22">
+      <c r="F11" s="21">
         <v>7999</v>
       </c>
     </row>
@@ -919,116 +935,148 @@
         <v>15</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="21">
+        <v>33</v>
+      </c>
+      <c r="C12" s="31">
+        <v>998.82</v>
+      </c>
+      <c r="D12" s="20">
         <v>1</v>
       </c>
       <c r="E12" s="18"/>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>998.82</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="21">
+        <v>21</v>
+      </c>
+      <c r="C13" s="31">
+        <v>35500</v>
+      </c>
+      <c r="D13" s="20">
         <v>2</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="22">
+      <c r="E13" s="33">
+        <f>(C13-(C13*(D13*0.2)))*0.1</f>
+        <v>2130</v>
+      </c>
+      <c r="F13" s="21">
         <v>1420</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="21">
+        <v>17</v>
+      </c>
+      <c r="C14" s="31">
+        <v>50000</v>
+      </c>
+      <c r="D14" s="20">
         <v>3</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="22">
+      <c r="E14" s="33">
+        <f>(C14-(C14*(D14*0.2)))*0.1</f>
+        <v>1999.9999999999998</v>
+      </c>
+      <c r="F14" s="21">
         <v>3000</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="21">
+        <v>18</v>
+      </c>
+      <c r="C15" s="31">
+        <v>44000</v>
+      </c>
+      <c r="D15" s="20">
         <v>3</v>
       </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="22">
+      <c r="E15" s="33">
+        <f>(C15-(C15*(D15*0.2)))*0.1</f>
+        <v>1759.9999999999998</v>
+      </c>
+      <c r="F15" s="21">
         <v>2640</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="21">
+      <c r="C16" s="31">
+        <v>50000</v>
+      </c>
+      <c r="D16" s="20">
         <v>2</v>
       </c>
-      <c r="E16" s="18"/>
-      <c r="F16" s="22">
+      <c r="E16" s="33">
+        <f>(C16-(C16*(D16*0.2)))*0.1</f>
+        <v>3000</v>
+      </c>
+      <c r="F16" s="21">
         <v>2000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="18"/>
-      <c r="D17" s="21">
+        <v>20</v>
+      </c>
+      <c r="C17" s="31">
+        <v>95000</v>
+      </c>
+      <c r="D17" s="20">
         <v>2</v>
       </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="22">
+      <c r="E17" s="33">
+        <f>(C17-(C17*(D17*0.2)))*0.1</f>
+        <v>5700</v>
+      </c>
+      <c r="F17" s="21">
         <v>3800</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="21">
+        <v>22</v>
+      </c>
+      <c r="C18" s="32">
+        <v>42000</v>
+      </c>
+      <c r="D18" s="20">
         <v>1</v>
       </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="22">
+      <c r="E18" s="33">
+        <f>(C18-(C18*(D18*0.2)))*0.1</f>
+        <v>3360</v>
+      </c>
+      <c r="F18" s="21">
         <v>840</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="11" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B19" s="11"/>
       <c r="C19" s="16"/>
@@ -1038,10 +1086,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1050,7 +1098,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>

</xml_diff>